<commit_message>
update metabolights GC template
add autosampler and guard column to match current requirements
</commit_message>
<xml_diff>
--- a/background information/MetaboLights/metabolights.xlsx
+++ b/background information/MetaboLights/metabolights.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stella Eggels\Documents\GitHub\Swate-templates\background information\MetaboLights\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stella Eggels\Documents\GitHub\swate-template-registry\background information\MetaboLights\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638B75B5-1A15-4869-A453-63331DA4B203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8A71E7-8DA3-416C-ABB6-B950FB423836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0096593A-FF03-4B73-8EDB-D9A655C6C356}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="72">
   <si>
     <t>NMR</t>
   </si>
@@ -206,9 +206,6 @@
     <t>derivatisation</t>
   </si>
   <si>
-    <t>last updated: 24.4.24</t>
-  </si>
-  <si>
     <t>NMR sample tube</t>
   </si>
   <si>
@@ -240,6 +237,21 @@
   </si>
   <si>
     <t>sample</t>
+  </si>
+  <si>
+    <t>last updated: 02.07.2025</t>
+  </si>
+  <si>
+    <t>guard column</t>
+  </si>
+  <si>
+    <t>autopsampler model</t>
+  </si>
+  <si>
+    <t>chromatography guard column model</t>
+  </si>
+  <si>
+    <t>chromatography autosampler model</t>
   </si>
 </sst>
 </file>
@@ -645,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ED24E31-6044-4BED-9FCF-483D3ECC09C5}">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -669,10 +681,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>27</v>
@@ -689,7 +701,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -697,7 +709,7 @@
         <v>26</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>26</v>
@@ -766,7 +778,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -774,7 +786,7 @@
         <v>42</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -782,7 +794,7 @@
         <v>6</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -790,7 +802,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -831,7 +843,7 @@
         <v>11</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>31</v>
@@ -865,7 +877,7 @@
         <v>13</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>33</v>
@@ -882,7 +894,7 @@
         <v>14</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>8</v>
@@ -899,7 +911,7 @@
         <v>15</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>9</v>
@@ -922,166 +934,182 @@
         <v>47</v>
       </c>
     </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="F25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="F26" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>35</v>
+        <v>68</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B30" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="H30" s="1" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="E29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="E30" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E31" s="1" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E32" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="E34" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="E35" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="H35" s="1" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B35" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B36" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B38" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B39" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B40" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B41" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B42" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B43" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add MetaboLights - Sample template
</commit_message>
<xml_diff>
--- a/background information/MetaboLights/metabolights.xlsx
+++ b/background information/MetaboLights/metabolights.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stella Eggels\Documents\GitHub\swate-template-registry\background information\MetaboLights\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8A71E7-8DA3-416C-ABB6-B950FB423836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF77FB4C-B4F1-4B71-B6D8-EE8A5B0641FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0096593A-FF03-4B73-8EDB-D9A655C6C356}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="83">
   <si>
     <t>NMR</t>
   </si>
@@ -252,6 +252,39 @@
   </si>
   <si>
     <t>chromatography autosampler model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample </t>
+  </si>
+  <si>
+    <t>Swate: Sample</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Organism</t>
+  </si>
+  <si>
+    <t>Organism part</t>
+  </si>
+  <si>
+    <t>Variant</t>
+  </si>
+  <si>
+    <t>Sample type</t>
+  </si>
+  <si>
+    <t>e.g. blank/control</t>
+  </si>
+  <si>
+    <t>sample collection</t>
+  </si>
+  <si>
+    <t>Variety</t>
+  </si>
+  <si>
+    <t>protocol ref</t>
   </si>
 </sst>
 </file>
@@ -657,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ED24E31-6044-4BED-9FCF-483D3ECC09C5}">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -670,10 +703,11 @@
     <col min="3" max="4" width="29.5546875" style="1" customWidth="1"/>
     <col min="5" max="6" width="29.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="29.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="11.5546875" style="1"/>
+    <col min="9" max="9" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>50</v>
       </c>
@@ -698,13 +732,25 @@
       <c r="H1" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>26</v>
       </c>
@@ -717,8 +763,22 @@
       <c r="F3" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
@@ -728,8 +788,14 @@
       <c r="F5" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
@@ -745,8 +811,17 @@
       <c r="G6" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E7" s="1" t="s">
         <v>29</v>
       </c>
@@ -756,8 +831,17 @@
       <c r="G7" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
@@ -767,13 +851,19 @@
       <c r="F8" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
@@ -781,7 +871,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>42</v>
       </c>
@@ -789,7 +879,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
@@ -797,7 +887,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
@@ -805,12 +895,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>9</v>
       </c>

</xml_diff>